<commit_message>
HOTFIX change date format in example
(cherry picked from commit f4766ec34b558cb00948a8eaa11ab729bf5a8619)
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example.xlsx
+++ b/apps/condo/public/meter-import-example.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\foxpro\condo\apps\condo\public\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409CAA9A-1EF3-4039-B142-BC6A7E6FDA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="1575" yWindow="4290" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Импортированный автор</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -30,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="26">
   <si>
     <t>Адрес</t>
   </si>
@@ -105,34 +114,34 @@
     <t>ГВС</t>
   </si>
   <si>
-    <t>20.01.2021</t>
-  </si>
-  <si>
-    <t>20.01.2015</t>
-  </si>
-  <si>
-    <t>21.01.2015</t>
-  </si>
-  <si>
     <t>ХВС</t>
   </si>
   <si>
     <t>г Москва, ул Тверская, д 2</t>
   </si>
   <si>
-    <t>20.02.2015</t>
-  </si>
-  <si>
-    <t>21.02.2015</t>
+    <t>2021-01-20</t>
+  </si>
+  <si>
+    <t>2021-01-21</t>
+  </si>
+  <si>
+    <t>2021-01-22</t>
+  </si>
+  <si>
+    <t>2021-01-23</t>
+  </si>
+  <si>
+    <t>2021-01-24</t>
+  </si>
+  <si>
+    <t>2021-01-25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -140,24 +149,29 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -251,72 +265,111 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -518,7 +571,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -537,7 +590,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -567,7 +620,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -593,7 +646,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -619,7 +672,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -645,7 +698,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -671,7 +724,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -697,7 +750,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -723,7 +776,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -749,7 +802,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -775,7 +828,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -788,9 +841,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -807,7 +866,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -826,7 +885,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -852,7 +911,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -878,7 +937,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -904,7 +963,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -930,7 +989,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -956,7 +1015,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -982,7 +1041,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1008,7 +1067,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1034,7 +1093,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1060,7 +1119,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1073,9 +1132,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1089,7 +1154,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1108,7 +1173,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1138,7 +1203,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1164,7 +1229,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1190,7 +1255,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1216,7 +1281,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1242,7 +1307,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1268,7 +1333,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1294,7 +1359,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1320,7 +1385,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1346,7 +1411,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1359,95 +1424,105 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.1719" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.67188" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3516" style="1" customWidth="1"/>
-    <col min="7" max="10" width="10.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6719" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.8516" style="1" customWidth="1"/>
-    <col min="14" max="14" width="22.1719" style="1" customWidth="1"/>
-    <col min="15" max="15" width="18.1719" style="1" customWidth="1"/>
-    <col min="16" max="16" width="23.5" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="1" customWidth="1"/>
+    <col min="7" max="10" width="10.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:16" ht="13.7" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="4">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="5">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="5">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="5">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="5">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="5">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="5">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="5">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="5">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="5">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="6">
+    <row r="2" spans="1:16" ht="13.7" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="7">
@@ -1456,7 +1531,7 @@
       <c r="C2" s="7">
         <v>111</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="7">
@@ -1475,27 +1550,27 @@
         <v>300</v>
       </c>
       <c r="J2" s="9"/>
-      <c r="K2" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="N2" t="s" s="5">
+      <c r="K2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O2" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="P2" t="s" s="5">
-        <v>20</v>
+      <c r="L2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="5">
+    <row r="3" spans="1:16" ht="13.7" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="8">
@@ -1504,7 +1579,7 @@
       <c r="C3" s="8">
         <v>111</v>
       </c>
-      <c r="D3" t="s" s="5">
+      <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="8">
@@ -1523,27 +1598,27 @@
         <v>400</v>
       </c>
       <c r="J3" s="9"/>
-      <c r="K3" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="L3" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="M3" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="N3" t="s" s="5">
+      <c r="K3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O3" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="P3" t="s" s="5">
-        <v>20</v>
+      <c r="L3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="5">
+    <row r="4" spans="1:16" ht="13.7" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="8">
@@ -1552,8 +1627,8 @@
       <c r="C4" s="8">
         <v>111</v>
       </c>
-      <c r="D4" t="s" s="5">
-        <v>21</v>
+      <c r="D4" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="E4" s="8">
         <v>2</v>
@@ -1571,27 +1646,27 @@
         <v>330</v>
       </c>
       <c r="J4" s="9"/>
-      <c r="K4" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="L4" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="M4" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="N4" t="s" s="5">
+      <c r="K4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O4" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="P4" t="s" s="5">
-        <v>20</v>
+      <c r="L4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="5">
+    <row r="5" spans="1:16" ht="13.7" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="8">
@@ -1600,8 +1675,8 @@
       <c r="C5" s="8">
         <v>111</v>
       </c>
-      <c r="D5" t="s" s="5">
-        <v>21</v>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="E5" s="8">
         <v>2</v>
@@ -1619,27 +1694,27 @@
         <v>405</v>
       </c>
       <c r="J5" s="9"/>
-      <c r="K5" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="L5" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="M5" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="N5" t="s" s="5">
+      <c r="K5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O5" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="P5" t="s" s="5">
-        <v>20</v>
+      <c r="L5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="5">
+    <row r="6" spans="1:16" ht="13.7" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="8">
@@ -1648,8 +1723,8 @@
       <c r="C6" s="8">
         <v>111</v>
       </c>
-      <c r="D6" t="s" s="5">
-        <v>21</v>
+      <c r="D6" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="E6" s="8">
         <v>2</v>
@@ -1667,28 +1742,28 @@
         <v>508</v>
       </c>
       <c r="J6" s="9"/>
-      <c r="K6" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="L6" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="M6" t="s" s="5">
+      <c r="K6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="13.7" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="N6" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="O6" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="P6" t="s" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="5">
-        <v>22</v>
       </c>
       <c r="B7" s="8">
         <v>2</v>
@@ -1696,7 +1771,7 @@
       <c r="C7" s="8">
         <v>222</v>
       </c>
-      <c r="D7" t="s" s="5">
+      <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="8">
@@ -1715,28 +1790,28 @@
         <v>304</v>
       </c>
       <c r="J7" s="9"/>
-      <c r="K7" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="L7" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="M7" t="s" s="5">
+      <c r="K7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N7" t="s" s="5">
+      <c r="O7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O7" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="P7" t="s" s="5">
-        <v>24</v>
+      <c r="P7" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" t="s" s="5">
-        <v>22</v>
+    <row r="8" spans="1:16" ht="13.7" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B8" s="8">
         <v>2</v>
@@ -1744,7 +1819,7 @@
       <c r="C8" s="8">
         <v>222</v>
       </c>
-      <c r="D8" t="s" s="5">
+      <c r="D8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="8">
@@ -1763,28 +1838,28 @@
         <v>503</v>
       </c>
       <c r="J8" s="9"/>
-      <c r="K8" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="L8" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="M8" t="s" s="5">
+      <c r="K8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N8" t="s" s="5">
+      <c r="O8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O8" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="P8" t="s" s="5">
-        <v>24</v>
+      <c r="P8" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" t="s" s="5">
-        <v>22</v>
+    <row r="9" spans="1:16" ht="13.7" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B9" s="8">
         <v>2</v>
@@ -1792,8 +1867,8 @@
       <c r="C9" s="8">
         <v>222</v>
       </c>
-      <c r="D9" t="s" s="5">
-        <v>21</v>
+      <c r="D9" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="E9" s="8">
         <v>22</v>
@@ -1811,28 +1886,28 @@
         <v>653</v>
       </c>
       <c r="J9" s="9"/>
-      <c r="K9" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="L9" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="M9" t="s" s="5">
+      <c r="K9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N9" t="s" s="5">
+      <c r="O9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O9" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="P9" t="s" s="5">
-        <v>24</v>
+      <c r="P9" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" t="s" s="5">
-        <v>22</v>
+    <row r="10" spans="1:16" ht="13.7" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B10" s="8">
         <v>2</v>
@@ -1840,8 +1915,8 @@
       <c r="C10" s="8">
         <v>222</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>21</v>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="E10" s="8">
         <v>22</v>
@@ -1859,32 +1934,32 @@
         <v>738</v>
       </c>
       <c r="J10" s="9"/>
-      <c r="K10" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="L10" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="M10" t="s" s="5">
+      <c r="K10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N10" t="s" s="5">
+      <c r="O10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O10" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="P10" t="s" s="5">
-        <v>24</v>
+      <c r="P10" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HOTFIX Add available meter types example
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example.xlsx
+++ b/apps/condo/public/meter-import-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\foxpro\condo\apps\condo\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409CAA9A-1EF3-4039-B142-BC6A7E6FDA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BA9B75-9B05-4C33-B1CE-4C4DE16AF42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="4290" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="2700" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
   <si>
     <t>Адрес</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>2021-01-25</t>
+  </si>
+  <si>
+    <t>ЭЛ</t>
+  </si>
+  <si>
+    <t>ТЕПЛО</t>
+  </si>
+  <si>
+    <t>ГАЗ</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1458,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1724,7 +1733,7 @@
         <v>111</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E6" s="8">
         <v>2</v>
@@ -1772,7 +1781,7 @@
         <v>222</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E7" s="8">
         <v>11</v>
@@ -1820,7 +1829,7 @@
         <v>222</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E8" s="8">
         <v>11</v>
@@ -1868,7 +1877,7 @@
         <v>222</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E9" s="8">
         <v>22</v>
@@ -1916,7 +1925,7 @@
         <v>222</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E10" s="8">
         <v>22</v>

</xml_diff>

<commit_message>
DOMA-1872 removed multi-tariff values for non-electricity meters from meter-import-example.xlsx
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example.xlsx
+++ b/apps/condo/public/meter-import-example.xlsx
@@ -1,31 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\foxpro\condo\apps\condo\public\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BA9B75-9B05-4C33-B1CE-4C4DE16AF42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="240" yWindow="2700" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Импортированный автор</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,7 +30,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Адрес</t>
   </si>
@@ -114,31 +105,31 @@
     <t>ГВС</t>
   </si>
   <si>
+    <t>2021-01-20</t>
+  </si>
+  <si>
+    <t>2021-01-21</t>
+  </si>
+  <si>
+    <t>2021-01-22</t>
+  </si>
+  <si>
+    <t>2021-01-23</t>
+  </si>
+  <si>
+    <t>2021-01-24</t>
+  </si>
+  <si>
+    <t>2021-01-25</t>
+  </si>
+  <si>
     <t>ХВС</t>
   </si>
   <si>
+    <t>ЭЛ</t>
+  </si>
+  <si>
     <t>г Москва, ул Тверская, д 2</t>
-  </si>
-  <si>
-    <t>2021-01-20</t>
-  </si>
-  <si>
-    <t>2021-01-21</t>
-  </si>
-  <si>
-    <t>2021-01-22</t>
-  </si>
-  <si>
-    <t>2021-01-23</t>
-  </si>
-  <si>
-    <t>2021-01-24</t>
-  </si>
-  <si>
-    <t>2021-01-25</t>
-  </si>
-  <si>
-    <t>ЭЛ</t>
   </si>
   <si>
     <t>ТЕПЛО</t>
@@ -150,7 +141,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -158,29 +152,24 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -274,111 +263,72 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -580,7 +530,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -599,7 +549,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -629,7 +579,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -655,7 +605,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -681,7 +631,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -707,7 +657,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -733,7 +683,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -759,7 +709,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -785,7 +735,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -811,7 +761,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -837,7 +787,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -850,15 +800,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -875,7 +819,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -894,7 +838,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -920,7 +864,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -946,7 +890,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -972,7 +916,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -998,7 +942,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1024,7 +968,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1050,7 +994,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1076,7 +1020,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1102,7 +1046,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1128,7 +1072,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1141,15 +1085,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1163,7 +1101,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1182,7 +1120,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1212,7 +1150,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1238,7 +1176,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1264,7 +1202,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1290,7 +1228,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1316,7 +1254,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1342,7 +1280,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1368,7 +1306,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1394,7 +1332,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1420,7 +1358,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1433,105 +1371,95 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.67188" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="1" customWidth="1"/>
-    <col min="7" max="10" width="10.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="23.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="14.42578125" style="1"/>
+    <col min="6" max="6" width="13.3516" style="1" customWidth="1"/>
+    <col min="7" max="10" width="10.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6719" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.8516" style="1" customWidth="1"/>
+    <col min="14" max="14" width="22.1719" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.1719" style="1" customWidth="1"/>
+    <col min="16" max="16" width="23.5" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13.7" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="13.7" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" t="s" s="5">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" t="s" s="5">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13.7" customHeight="1">
-      <c r="A2" s="6" t="s">
+    <row r="2" ht="13.7" customHeight="1">
+      <c r="A2" t="s" s="6">
         <v>16</v>
       </c>
       <c r="B2" s="7">
@@ -1540,46 +1468,42 @@
       <c r="C2" s="7">
         <v>111</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s" s="6">
         <v>17</v>
       </c>
       <c r="E2" s="7">
         <v>1</v>
       </c>
       <c r="F2" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" s="8">
         <v>100</v>
       </c>
-      <c r="H2" s="8">
-        <v>200</v>
-      </c>
-      <c r="I2" s="8">
-        <v>300</v>
-      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
       <c r="J2" s="9"/>
-      <c r="K2" s="10" t="s">
+      <c r="K2" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="N2" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="O2" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="P2" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="O2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="3" spans="1:16" ht="13.7" customHeight="1">
-      <c r="A3" s="5" t="s">
+    <row r="3" ht="13.7" customHeight="1">
+      <c r="A3" t="s" s="5">
         <v>16</v>
       </c>
       <c r="B3" s="8">
@@ -1588,46 +1512,42 @@
       <c r="C3" s="8">
         <v>111</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s" s="5">
         <v>17</v>
       </c>
       <c r="E3" s="8">
         <v>1</v>
       </c>
       <c r="F3" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3" s="8">
         <v>200</v>
       </c>
-      <c r="H3" s="8">
-        <v>300</v>
-      </c>
-      <c r="I3" s="8">
-        <v>400</v>
-      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="9"/>
-      <c r="K3" s="10" t="s">
+      <c r="K3" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="N3" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="O3" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="P3" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="O3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="4" spans="1:16" ht="13.7" customHeight="1">
-      <c r="A4" s="5" t="s">
+    <row r="4" ht="13.7" customHeight="1">
+      <c r="A4" t="s" s="5">
         <v>16</v>
       </c>
       <c r="B4" s="8">
@@ -1636,46 +1556,42 @@
       <c r="C4" s="8">
         <v>111</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
+      <c r="D4" t="s" s="5">
+        <v>24</v>
       </c>
       <c r="E4" s="8">
         <v>2</v>
       </c>
       <c r="F4" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G4" s="8">
         <v>110</v>
       </c>
-      <c r="H4" s="8">
-        <v>220</v>
-      </c>
-      <c r="I4" s="8">
-        <v>330</v>
-      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="10" t="s">
+      <c r="K4" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="N4" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="O4" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="P4" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="O4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="5" spans="1:16" ht="13.7" customHeight="1">
-      <c r="A5" s="5" t="s">
+    <row r="5" ht="13.7" customHeight="1">
+      <c r="A5" t="s" s="5">
         <v>16</v>
       </c>
       <c r="B5" s="8">
@@ -1684,46 +1600,42 @@
       <c r="C5" s="8">
         <v>111</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
+      <c r="D5" t="s" s="5">
+        <v>24</v>
       </c>
       <c r="E5" s="8">
         <v>2</v>
       </c>
       <c r="F5" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G5" s="8">
         <v>300</v>
       </c>
-      <c r="H5" s="8">
-        <v>350</v>
-      </c>
-      <c r="I5" s="8">
-        <v>405</v>
-      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
       <c r="J5" s="9"/>
-      <c r="K5" s="10" t="s">
+      <c r="K5" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="N5" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="O5" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="P5" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="O5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="6" spans="1:16" ht="13.7" customHeight="1">
-      <c r="A6" s="5" t="s">
+    <row r="6" ht="13.7" customHeight="1">
+      <c r="A6" t="s" s="5">
         <v>16</v>
       </c>
       <c r="B6" s="8">
@@ -1732,8 +1644,8 @@
       <c r="C6" s="8">
         <v>111</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>26</v>
+      <c r="D6" t="s" s="5">
+        <v>25</v>
       </c>
       <c r="E6" s="8">
         <v>2</v>
@@ -1751,28 +1663,28 @@
         <v>508</v>
       </c>
       <c r="J6" s="9"/>
-      <c r="K6" s="10" t="s">
+      <c r="K6" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="N6" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="O6" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="P6" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="O6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="7" spans="1:16" ht="13.7" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>19</v>
+    <row r="7" ht="13.7" customHeight="1">
+      <c r="A7" t="s" s="5">
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <v>2</v>
@@ -1780,8 +1692,8 @@
       <c r="C7" s="8">
         <v>222</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>26</v>
+      <c r="D7" t="s" s="5">
+        <v>25</v>
       </c>
       <c r="E7" s="8">
         <v>11</v>
@@ -1799,28 +1711,28 @@
         <v>304</v>
       </c>
       <c r="J7" s="9"/>
-      <c r="K7" s="10" t="s">
+      <c r="K7" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="M7" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="N7" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="O7" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="P7" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="O7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="8" spans="1:16" ht="13.7" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
+    <row r="8" ht="13.7" customHeight="1">
+      <c r="A8" t="s" s="5">
+        <v>26</v>
       </c>
       <c r="B8" s="8">
         <v>2</v>
@@ -1828,47 +1740,43 @@
       <c r="C8" s="8">
         <v>222</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" t="s" s="5">
         <v>27</v>
       </c>
       <c r="E8" s="8">
         <v>11</v>
       </c>
       <c r="F8" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G8" s="8">
         <v>238</v>
       </c>
-      <c r="H8" s="8">
-        <v>450</v>
-      </c>
-      <c r="I8" s="8">
-        <v>503</v>
-      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="10" t="s">
+      <c r="K8" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="M8" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="N8" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="O8" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="P8" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="O8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P8" s="10" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="9" spans="1:16" ht="13.7" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>19</v>
+    <row r="9" ht="13.7" customHeight="1">
+      <c r="A9" t="s" s="5">
+        <v>26</v>
       </c>
       <c r="B9" s="8">
         <v>2</v>
@@ -1876,47 +1784,43 @@
       <c r="C9" s="8">
         <v>222</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" t="s" s="5">
         <v>27</v>
       </c>
       <c r="E9" s="8">
         <v>22</v>
       </c>
       <c r="F9" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9" s="8">
         <v>294</v>
       </c>
-      <c r="H9" s="8">
-        <v>483</v>
-      </c>
-      <c r="I9" s="8">
-        <v>653</v>
-      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="10" t="s">
+      <c r="K9" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="M9" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="N9" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="O9" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="P9" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="O9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P9" s="10" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="10" spans="1:16" ht="13.7" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>19</v>
+    <row r="10" ht="13.7" customHeight="1">
+      <c r="A10" t="s" s="5">
+        <v>26</v>
       </c>
       <c r="B10" s="8">
         <v>2</v>
@@ -1924,51 +1828,47 @@
       <c r="C10" s="8">
         <v>222</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s" s="5">
         <v>28</v>
       </c>
       <c r="E10" s="8">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F10" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10" s="8">
         <v>338</v>
       </c>
-      <c r="H10" s="8">
-        <v>683</v>
-      </c>
-      <c r="I10" s="8">
-        <v>738</v>
-      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="10" t="s">
+      <c r="K10" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="L10" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="M10" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="N10" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="O10" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="P10" t="s" s="5">
         <v>23</v>
-      </c>
-      <c r="O10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P10" s="10" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DOMA-1872 removed cell comments from meter-import-example.xlsx
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example.xlsx
+++ b/apps/condo/public/meter-import-example.xlsx
@@ -10,44 +10,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Импортированный автор</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-          </rPr>
-          <t>Импортированный автор:
-Адрес вместе с квартирой
-	-Антон Алёшин</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Helvetica Neue"/>
-          </rPr>
-          <t>Импортированный автор:
-пОверки
-	-Антон Алёшин</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
@@ -145,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -165,11 +127,6 @@
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="4">
@@ -321,10 +278,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1868,7 +1821,5 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DOMA-1858 new column "Reading submission date" for import of meter readings
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example.xlsx
+++ b/apps/condo/public/meter-import-example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>Адрес</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Показание 4</t>
   </si>
   <si>
+    <t>Дата передачи показаний</t>
+  </si>
+  <si>
     <t>Дата поверки</t>
   </si>
   <si>
@@ -67,6 +70,9 @@
     <t>ГВС</t>
   </si>
   <si>
+    <t>2021-12-20</t>
+  </si>
+  <si>
     <t>2021-01-20</t>
   </si>
   <si>
@@ -92,6 +98,9 @@
   </si>
   <si>
     <t>г Москва, ул Тверская, д 2</t>
+  </si>
+  <si>
+    <t>2021-12-21</t>
   </si>
   <si>
     <t>ТЕПЛО</t>
@@ -1339,7 +1348,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1352,13 +1361,14 @@
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.3516" style="1" customWidth="1"/>
     <col min="7" max="10" width="10.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6719" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.8516" style="1" customWidth="1"/>
-    <col min="14" max="14" width="22.1719" style="1" customWidth="1"/>
-    <col min="15" max="15" width="18.1719" style="1" customWidth="1"/>
-    <col min="16" max="16" width="23.5" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.8516" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.6719" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.8516" style="1" customWidth="1"/>
+    <col min="15" max="15" width="22.1719" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.1719" style="1" customWidth="1"/>
+    <col min="17" max="17" width="23.5" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.7" customHeight="1">
@@ -1410,10 +1420,13 @@
       <c r="P1" t="s" s="5">
         <v>15</v>
       </c>
+      <c r="Q1" t="s" s="5">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" ht="13.7" customHeight="1">
       <c r="A2" t="s" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>
@@ -1422,7 +1435,7 @@
         <v>111</v>
       </c>
       <c r="D2" t="s" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="7">
         <v>1</v>
@@ -1437,27 +1450,30 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" t="s" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N2" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O2" t="s" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P2" t="s" s="5">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="3" ht="13.7" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -1466,7 +1482,7 @@
         <v>111</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="8">
         <v>1</v>
@@ -1481,27 +1497,30 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" t="s" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L3" t="s" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M3" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N3" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O3" t="s" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P3" t="s" s="5">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="Q3" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="4" ht="13.7" customHeight="1">
       <c r="A4" t="s" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="8">
         <v>1</v>
@@ -1510,7 +1529,7 @@
         <v>111</v>
       </c>
       <c r="D4" t="s" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E4" s="8">
         <v>2</v>
@@ -1525,27 +1544,30 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" t="s" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M4" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N4" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O4" t="s" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P4" t="s" s="5">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="5" ht="13.7" customHeight="1">
       <c r="A5" t="s" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="8">
         <v>1</v>
@@ -1554,7 +1576,7 @@
         <v>111</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5" s="8">
         <v>2</v>
@@ -1569,27 +1591,30 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" t="s" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L5" t="s" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M5" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N5" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O5" t="s" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P5" t="s" s="5">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="Q5" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="6" ht="13.7" customHeight="1">
       <c r="A6" t="s" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="8">
         <v>1</v>
@@ -1598,7 +1623,7 @@
         <v>111</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E6" s="8">
         <v>2</v>
@@ -1617,27 +1642,30 @@
       </c>
       <c r="J6" s="9"/>
       <c r="K6" t="s" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L6" t="s" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M6" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N6" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O6" t="s" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P6" t="s" s="5">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="Q6" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="7" ht="13.7" customHeight="1">
       <c r="A7" t="s" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" s="8">
         <v>2</v>
@@ -1646,7 +1674,7 @@
         <v>222</v>
       </c>
       <c r="D7" t="s" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E7" s="8">
         <v>11</v>
@@ -1665,27 +1693,30 @@
       </c>
       <c r="J7" s="9"/>
       <c r="K7" t="s" s="5">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="L7" t="s" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M7" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N7" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O7" t="s" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P7" t="s" s="5">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="Q7" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="8" ht="13.7" customHeight="1">
       <c r="A8" t="s" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8">
         <v>2</v>
@@ -1694,7 +1725,7 @@
         <v>222</v>
       </c>
       <c r="D8" t="s" s="5">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E8" s="8">
         <v>11</v>
@@ -1709,27 +1740,30 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" t="s" s="5">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="L8" t="s" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M8" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N8" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O8" t="s" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P8" t="s" s="5">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="Q8" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="9" ht="13.7" customHeight="1">
       <c r="A9" t="s" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B9" s="8">
         <v>2</v>
@@ -1738,7 +1772,7 @@
         <v>222</v>
       </c>
       <c r="D9" t="s" s="5">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E9" s="8">
         <v>22</v>
@@ -1753,27 +1787,30 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" t="s" s="5">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="L9" t="s" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M9" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N9" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O9" t="s" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P9" t="s" s="5">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="Q9" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="10" ht="13.7" customHeight="1">
       <c r="A10" t="s" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" s="8">
         <v>2</v>
@@ -1782,7 +1819,7 @@
         <v>222</v>
       </c>
       <c r="D10" t="s" s="5">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E10" s="8">
         <v>33</v>
@@ -1797,22 +1834,25 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" t="s" s="5">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="L10" t="s" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M10" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N10" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O10" t="s" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P10" t="s" s="5">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="Q10" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DOMA-1858 parsing of "Reading submission date" column value either in "YYYY-MM-DD" or "YYYY-MM-DD" format
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example.xlsx
+++ b/apps/condo/public/meter-import-example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>Адрес</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>ХВС</t>
+  </si>
+  <si>
+    <t>2021-12</t>
   </si>
   <si>
     <t>ЭЛ</t>
@@ -1591,7 +1594,7 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" t="s" s="5">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="L5" t="s" s="5">
         <v>20</v>
@@ -1623,7 +1626,7 @@
         <v>111</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="8">
         <v>2</v>
@@ -1665,7 +1668,7 @@
     </row>
     <row r="7" ht="13.7" customHeight="1">
       <c r="A7" t="s" s="5">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="8">
         <v>2</v>
@@ -1674,7 +1677,7 @@
         <v>222</v>
       </c>
       <c r="D7" t="s" s="5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="8">
         <v>11</v>
@@ -1693,7 +1696,7 @@
       </c>
       <c r="J7" s="9"/>
       <c r="K7" t="s" s="5">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s" s="5">
         <v>20</v>
@@ -1716,7 +1719,7 @@
     </row>
     <row r="8" ht="13.7" customHeight="1">
       <c r="A8" t="s" s="5">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="8">
         <v>2</v>
@@ -1725,7 +1728,7 @@
         <v>222</v>
       </c>
       <c r="D8" t="s" s="5">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="8">
         <v>11</v>
@@ -1740,7 +1743,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" t="s" s="5">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L8" t="s" s="5">
         <v>20</v>
@@ -1763,7 +1766,7 @@
     </row>
     <row r="9" ht="13.7" customHeight="1">
       <c r="A9" t="s" s="5">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8">
         <v>2</v>
@@ -1772,7 +1775,7 @@
         <v>222</v>
       </c>
       <c r="D9" t="s" s="5">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="8">
         <v>22</v>
@@ -1787,7 +1790,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" t="s" s="5">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L9" t="s" s="5">
         <v>20</v>
@@ -1810,7 +1813,7 @@
     </row>
     <row r="10" ht="13.7" customHeight="1">
       <c r="A10" t="s" s="5">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="8">
         <v>2</v>
@@ -1819,7 +1822,7 @@
         <v>222</v>
       </c>
       <c r="D10" t="s" s="5">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="8">
         <v>33</v>
@@ -1834,7 +1837,7 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" t="s" s="5">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L10" t="s" s="5">
         <v>20</v>

</xml_diff>

<commit_message>
DOMA-1851 used "custom" column type for "readingSubmissionDate" column
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example.xlsx
+++ b/apps/condo/public/meter-import-example.xlsx
@@ -73,9 +73,6 @@
     <t>2021-12-20</t>
   </si>
   <si>
-    <t>2021-01-20</t>
-  </si>
-  <si>
     <t>2021-01-21</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>ЭЛ</t>
+  </si>
+  <si>
+    <t>2021-11-20</t>
   </si>
   <si>
     <t>г Москва, ул Тверская, д 2</t>
@@ -116,8 +116,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="d.mm.yyyy"/>
+    <numFmt numFmtId="60" formatCode="dd.mm.yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -236,7 +238,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -265,6 +267,12 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1351,7 +1359,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1455,23 +1463,23 @@
       <c r="K2" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="L2" t="s" s="5">
+      <c r="L2" s="10">
+        <v>44216</v>
+      </c>
+      <c r="M2" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="M2" t="s" s="5">
+      <c r="N2" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="N2" t="s" s="5">
+      <c r="O2" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="O2" t="s" s="5">
+      <c r="P2" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="P2" t="s" s="5">
+      <c r="Q2" t="s" s="5">
         <v>24</v>
-      </c>
-      <c r="Q2" t="s" s="5">
-        <v>25</v>
       </c>
     </row>
     <row r="3" ht="13.7" customHeight="1">
@@ -1502,23 +1510,23 @@
       <c r="K3" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="L3" t="s" s="5">
+      <c r="L3" s="10">
+        <v>44216</v>
+      </c>
+      <c r="M3" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="M3" t="s" s="5">
+      <c r="N3" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="N3" t="s" s="5">
+      <c r="O3" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="O3" t="s" s="5">
+      <c r="P3" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="P3" t="s" s="5">
+      <c r="Q3" t="s" s="5">
         <v>24</v>
-      </c>
-      <c r="Q3" t="s" s="5">
-        <v>25</v>
       </c>
     </row>
     <row r="4" ht="13.7" customHeight="1">
@@ -1532,7 +1540,7 @@
         <v>111</v>
       </c>
       <c r="D4" t="s" s="5">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="8">
         <v>2</v>
@@ -1549,23 +1557,23 @@
       <c r="K4" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="L4" t="s" s="5">
+      <c r="L4" s="10">
+        <v>44216</v>
+      </c>
+      <c r="M4" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="M4" t="s" s="5">
+      <c r="N4" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="N4" t="s" s="5">
+      <c r="O4" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="O4" t="s" s="5">
+      <c r="P4" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="P4" t="s" s="5">
+      <c r="Q4" t="s" s="5">
         <v>24</v>
-      </c>
-      <c r="Q4" t="s" s="5">
-        <v>25</v>
       </c>
     </row>
     <row r="5" ht="13.7" customHeight="1">
@@ -1579,7 +1587,7 @@
         <v>111</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="8">
         <v>2</v>
@@ -1594,25 +1602,25 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" t="s" s="5">
-        <v>27</v>
-      </c>
-      <c r="L5" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="L5" s="10">
+        <v>44216</v>
+      </c>
+      <c r="M5" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="M5" t="s" s="5">
+      <c r="N5" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="N5" t="s" s="5">
+      <c r="O5" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="O5" t="s" s="5">
+      <c r="P5" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="P5" t="s" s="5">
+      <c r="Q5" t="s" s="5">
         <v>24</v>
-      </c>
-      <c r="Q5" t="s" s="5">
-        <v>25</v>
       </c>
     </row>
     <row r="6" ht="13.7" customHeight="1">
@@ -1626,7 +1634,7 @@
         <v>111</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="8">
         <v>2</v>
@@ -1645,76 +1653,76 @@
       </c>
       <c r="J6" s="9"/>
       <c r="K6" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="L6" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="L6" s="10">
+        <v>44216</v>
+      </c>
+      <c r="M6" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="M6" t="s" s="5">
+      <c r="N6" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="N6" t="s" s="5">
+      <c r="O6" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="O6" t="s" s="5">
+      <c r="P6" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="P6" t="s" s="5">
+      <c r="Q6" t="s" s="5">
         <v>24</v>
-      </c>
-      <c r="Q6" t="s" s="5">
-        <v>25</v>
       </c>
     </row>
     <row r="7" ht="13.7" customHeight="1">
       <c r="A7" t="s" s="5">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8">
+        <v>111</v>
+      </c>
+      <c r="D7" t="s" s="5">
+        <v>27</v>
+      </c>
+      <c r="E7" s="8">
         <v>2</v>
-      </c>
-      <c r="C7" s="8">
-        <v>222</v>
-      </c>
-      <c r="D7" t="s" s="5">
-        <v>28</v>
-      </c>
-      <c r="E7" s="8">
-        <v>11</v>
       </c>
       <c r="F7" s="8">
         <v>3</v>
       </c>
       <c r="G7" s="8">
-        <v>150</v>
+        <v>673</v>
       </c>
       <c r="H7" s="8">
-        <v>238</v>
+        <v>573</v>
       </c>
       <c r="I7" s="8">
-        <v>304</v>
+        <v>584</v>
       </c>
       <c r="J7" s="9"/>
-      <c r="K7" t="s" s="5">
-        <v>30</v>
-      </c>
-      <c r="L7" t="s" s="5">
+      <c r="K7" s="11">
+        <v>44550</v>
+      </c>
+      <c r="L7" s="10">
+        <v>44216</v>
+      </c>
+      <c r="M7" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="M7" t="s" s="5">
+      <c r="N7" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="N7" t="s" s="5">
+      <c r="O7" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="O7" t="s" s="5">
+      <c r="P7" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="P7" t="s" s="5">
+      <c r="Q7" t="s" s="5">
         <v>24</v>
-      </c>
-      <c r="Q7" t="s" s="5">
-        <v>25</v>
       </c>
     </row>
     <row r="8" ht="13.7" customHeight="1">
@@ -1728,40 +1736,44 @@
         <v>222</v>
       </c>
       <c r="D8" t="s" s="5">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E8" s="8">
         <v>11</v>
       </c>
       <c r="F8" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" s="8">
+        <v>150</v>
+      </c>
+      <c r="H8" s="8">
         <v>238</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="I8" s="8">
+        <v>304</v>
+      </c>
       <c r="J8" s="9"/>
       <c r="K8" t="s" s="5">
         <v>30</v>
       </c>
-      <c r="L8" t="s" s="5">
+      <c r="L8" s="10">
+        <v>44216</v>
+      </c>
+      <c r="M8" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="M8" t="s" s="5">
+      <c r="N8" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="N8" t="s" s="5">
+      <c r="O8" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="O8" t="s" s="5">
+      <c r="P8" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="P8" t="s" s="5">
+      <c r="Q8" t="s" s="5">
         <v>24</v>
-      </c>
-      <c r="Q8" t="s" s="5">
-        <v>25</v>
       </c>
     </row>
     <row r="9" ht="13.7" customHeight="1">
@@ -1778,37 +1790,37 @@
         <v>31</v>
       </c>
       <c r="E9" s="8">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F9" s="8">
         <v>1</v>
       </c>
       <c r="G9" s="8">
-        <v>294</v>
+        <v>238</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" t="s" s="5">
-        <v>27</v>
-      </c>
-      <c r="L9" t="s" s="5">
+        <v>30</v>
+      </c>
+      <c r="L9" s="10">
+        <v>44216</v>
+      </c>
+      <c r="M9" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="M9" t="s" s="5">
+      <c r="N9" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="N9" t="s" s="5">
+      <c r="O9" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="O9" t="s" s="5">
+      <c r="P9" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="P9" t="s" s="5">
+      <c r="Q9" t="s" s="5">
         <v>24</v>
-      </c>
-      <c r="Q9" t="s" s="5">
-        <v>25</v>
       </c>
     </row>
     <row r="10" ht="13.7" customHeight="1">
@@ -1822,40 +1834,87 @@
         <v>222</v>
       </c>
       <c r="D10" t="s" s="5">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="8">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F10" s="8">
         <v>1</v>
       </c>
       <c r="G10" s="8">
-        <v>338</v>
+        <v>294</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" t="s" s="5">
-        <v>27</v>
-      </c>
-      <c r="L10" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="L10" s="10">
+        <v>44216</v>
+      </c>
+      <c r="M10" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="M10" t="s" s="5">
+      <c r="N10" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="N10" t="s" s="5">
+      <c r="O10" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="O10" t="s" s="5">
+      <c r="P10" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="P10" t="s" s="5">
+      <c r="Q10" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="Q10" t="s" s="5">
-        <v>25</v>
+    </row>
+    <row r="11" ht="13.7" customHeight="1">
+      <c r="A11" t="s" s="5">
+        <v>29</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2</v>
+      </c>
+      <c r="C11" s="8">
+        <v>222</v>
+      </c>
+      <c r="D11" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="E11" s="8">
+        <v>33</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8">
+        <v>338</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="L11" s="10">
+        <v>44216</v>
+      </c>
+      <c r="M11" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="O11" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="P11" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="Q11" t="s" s="5">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DOMA-2143 Make one of values required and changed meter example
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example.xlsx
+++ b/apps/condo/public/meter-import-example.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsavelev/WebstormProjects/condo/apps/condo/public/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C2CC39-0E47-E141-ABF4-A038EB6E0DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
   <si>
     <t>Адрес</t>
   </si>
@@ -115,35 +124,36 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="d.mm.yyyy"/>
-    <numFmt numFmtId="60" formatCode="dd.mm.yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="d\.mm\.yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +170,18 @@
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -234,47 +256,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -283,25 +288,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -503,7 +568,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -522,7 +587,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -552,7 +617,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -578,7 +643,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -604,7 +669,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -630,7 +695,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -656,7 +721,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -682,7 +747,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -708,7 +773,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -734,7 +799,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -760,7 +825,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -773,9 +838,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -792,7 +863,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -811,7 +882,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -837,7 +908,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -863,7 +934,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -889,7 +960,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -915,7 +986,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -941,7 +1012,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -967,7 +1038,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -993,7 +1064,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1019,7 +1090,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1045,7 +1116,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1058,9 +1129,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1074,7 +1151,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1093,7 +1170,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1123,7 +1200,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1149,7 +1226,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1175,7 +1252,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1201,7 +1278,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1304,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1253,7 +1330,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1279,7 +1356,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1305,7 +1382,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,7 +1408,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1344,582 +1421,592 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.1719" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.67188" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="1" customWidth="1"/>
     <col min="7" max="10" width="10.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.8516" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6719" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.8516" style="1" customWidth="1"/>
-    <col min="15" max="15" width="22.1719" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.1719" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="22.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.1640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="23.5" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.7" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="4">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="5">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="5">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="5">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="5">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="5">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="5">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="5">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="5">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="5">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="5">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" ht="13.7" customHeight="1">
-      <c r="A2" t="s" s="6">
+    <row r="2" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>111</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>1</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>100</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" t="s" s="5">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="9">
         <v>44216</v>
       </c>
-      <c r="M2" t="s" s="5">
+      <c r="M2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N2" t="s" s="5">
+      <c r="N2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O2" t="s" s="5">
+      <c r="O2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P2" t="s" s="5">
+      <c r="P2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" t="s" s="5">
+      <c r="Q2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" ht="13.7" customHeight="1">
-      <c r="A3" t="s" s="5">
+    <row r="3" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>111</v>
       </c>
-      <c r="D3" t="s" s="5">
+      <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>1</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>1</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>200</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" t="s" s="5">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="9">
         <v>44216</v>
       </c>
-      <c r="M3" t="s" s="5">
+      <c r="M3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N3" t="s" s="5">
+      <c r="N3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O3" t="s" s="5">
+      <c r="O3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P3" t="s" s="5">
+      <c r="P3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" t="s" s="5">
+      <c r="Q3" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" ht="13.7" customHeight="1">
-      <c r="A4" t="s" s="5">
+    <row r="4" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>111</v>
       </c>
-      <c r="D4" t="s" s="5">
+      <c r="D4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>2</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>110</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" t="s" s="5">
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="9">
         <v>44216</v>
       </c>
-      <c r="M4" t="s" s="5">
+      <c r="M4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N4" t="s" s="5">
+      <c r="N4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O4" t="s" s="5">
+      <c r="O4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P4" t="s" s="5">
+      <c r="P4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" t="s" s="5">
+      <c r="Q4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" ht="13.7" customHeight="1">
-      <c r="A5" t="s" s="5">
+    <row r="5" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>111</v>
       </c>
-      <c r="D5" t="s" s="5">
+      <c r="D5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>2</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>300</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" t="s" s="5">
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="9">
         <v>44216</v>
       </c>
-      <c r="M5" t="s" s="5">
+      <c r="M5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N5" t="s" s="5">
+      <c r="N5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O5" t="s" s="5">
+      <c r="O5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P5" t="s" s="5">
+      <c r="P5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" t="s" s="5">
+      <c r="Q5" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" ht="13.7" customHeight="1">
-      <c r="A6" t="s" s="5">
+    <row r="6" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>111</v>
       </c>
-      <c r="D6" t="s" s="5">
+      <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>2</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>3</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>564</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>483</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>508</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" t="s" s="5">
+      <c r="J6" s="8"/>
+      <c r="K6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="9">
         <v>44216</v>
       </c>
-      <c r="M6" t="s" s="5">
+      <c r="M6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N6" t="s" s="5">
+      <c r="N6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O6" t="s" s="5">
+      <c r="O6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P6" t="s" s="5">
+      <c r="P6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q6" t="s" s="5">
+      <c r="Q6" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" ht="13.7" customHeight="1">
-      <c r="A7" t="s" s="5">
+    <row r="7" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>1</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>111</v>
       </c>
-      <c r="D7" t="s" s="5">
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>2</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>3</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>673</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <v>573</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>584</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="11">
+      <c r="J7" s="8"/>
+      <c r="K7" s="10">
         <v>44550</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="9">
         <v>44216</v>
       </c>
-      <c r="M7" t="s" s="5">
+      <c r="M7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N7" t="s" s="5">
+      <c r="N7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O7" t="s" s="5">
+      <c r="O7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P7" t="s" s="5">
+      <c r="P7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q7" t="s" s="5">
+      <c r="Q7" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" ht="13.7" customHeight="1">
-      <c r="A8" t="s" s="5">
+    <row r="8" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>2</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>222</v>
       </c>
-      <c r="D8" t="s" s="5">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>11</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>3</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>150</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>238</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <v>304</v>
       </c>
-      <c r="J8" s="9"/>
-      <c r="K8" t="s" s="5">
+      <c r="J8" s="8"/>
+      <c r="K8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="9">
         <v>44216</v>
       </c>
-      <c r="M8" t="s" s="5">
+      <c r="M8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N8" t="s" s="5">
+      <c r="N8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O8" t="s" s="5">
+      <c r="O8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P8" t="s" s="5">
+      <c r="P8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" t="s" s="5">
+      <c r="Q8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" ht="13.7" customHeight="1">
-      <c r="A9" t="s" s="5">
+    <row r="9" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>2</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>222</v>
       </c>
-      <c r="D9" t="s" s="5">
+      <c r="D9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>11</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>1</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>238</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" t="s" s="5">
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="9">
         <v>44216</v>
       </c>
-      <c r="M9" t="s" s="5">
+      <c r="M9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N9" t="s" s="5">
+      <c r="N9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O9" t="s" s="5">
+      <c r="O9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P9" t="s" s="5">
+      <c r="P9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q9" t="s" s="5">
+      <c r="Q9" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" ht="13.7" customHeight="1">
-      <c r="A10" t="s" s="5">
+    <row r="10" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>2</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>222</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>22</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>1</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>294</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" t="s" s="5">
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="9">
         <v>44216</v>
       </c>
-      <c r="M10" t="s" s="5">
+      <c r="M10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N10" t="s" s="5">
+      <c r="N10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O10" t="s" s="5">
+      <c r="O10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P10" t="s" s="5">
+      <c r="P10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q10" t="s" s="5">
+      <c r="Q10" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" ht="13.7" customHeight="1">
-      <c r="A11" t="s" s="5">
+    <row r="11" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>2</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>222</v>
       </c>
-      <c r="D11" t="s" s="5">
+      <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>33</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>1</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>338</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" t="s" s="5">
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="9">
         <v>44216</v>
       </c>
-      <c r="M11" t="s" s="5">
+      <c r="M11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N11" t="s" s="5">
+      <c r="N11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O11" t="s" s="5">
+      <c r="O11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P11" t="s" s="5">
+      <c r="P11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q11" t="s" s="5">
+      <c r="Q11" s="4" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
DOMA-3110 added unitType to meter import
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example.xlsx
+++ b/apps/condo/public/meter-import-example.xlsx
@@ -1,79 +1,76 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsavelev/WebstormProjects/condo/apps/condo/public/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C2CC39-0E47-E141-ABF4-A038EB6E0DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>Адрес</t>
   </si>
   <si>
+    <t>Помещение</t>
+  </si>
+  <si>
+    <t>Тип помещения</t>
+  </si>
+  <si>
+    <t>ЛС</t>
+  </si>
+  <si>
+    <t>Тип счетчика</t>
+  </si>
+  <si>
+    <t>№ счетчика</t>
+  </si>
+  <si>
+    <t>Кол-во тарифов</t>
+  </si>
+  <si>
+    <t>Показание 1</t>
+  </si>
+  <si>
+    <t>Показание 2</t>
+  </si>
+  <si>
+    <t>Показание 3</t>
+  </si>
+  <si>
+    <t>Показание 4</t>
+  </si>
+  <si>
+    <t>Дата передачи показаний</t>
+  </si>
+  <si>
+    <t>Дата поверки</t>
+  </si>
+  <si>
+    <t>Дата следующей поверки</t>
+  </si>
+  <si>
+    <t>Дата установки</t>
+  </si>
+  <si>
+    <t>Дата ввода в эксплуатацию</t>
+  </si>
+  <si>
+    <t>Дата опломбирования</t>
+  </si>
+  <si>
+    <t>Дата контрольных показаний</t>
+  </si>
+  <si>
+    <t>г Москва, ул Тверская, д 1</t>
+  </si>
+  <si>
     <t>Квартира</t>
-  </si>
-  <si>
-    <t>ЛС</t>
-  </si>
-  <si>
-    <t>Тип счетчика</t>
-  </si>
-  <si>
-    <t>№ счетчика</t>
-  </si>
-  <si>
-    <t>Кол-во тарифов</t>
-  </si>
-  <si>
-    <t>Показание 1</t>
-  </si>
-  <si>
-    <t>Показание 2</t>
-  </si>
-  <si>
-    <t>Показание 3</t>
-  </si>
-  <si>
-    <t>Показание 4</t>
-  </si>
-  <si>
-    <t>Дата передачи показаний</t>
-  </si>
-  <si>
-    <t>Дата поверки</t>
-  </si>
-  <si>
-    <t>Дата следующей поверки</t>
-  </si>
-  <si>
-    <t>Дата установки</t>
-  </si>
-  <si>
-    <t>Дата ввода в эксплуатацию</t>
-  </si>
-  <si>
-    <t>Дата опломбирования</t>
-  </si>
-  <si>
-    <t>Дата контрольных показаний</t>
-  </si>
-  <si>
-    <t>г Москва, ул Тверская, д 1</t>
   </si>
   <si>
     <t>ГВС</t>
@@ -124,36 +121,35 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="d\.mm\.yyyy"/>
-    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="d&quot;.&quot;mm&quot;.&quot;yyyy"/>
+    <numFmt numFmtId="60" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,20 +164,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
@@ -256,30 +246,53 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -288,85 +301,26 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="fffbbc04"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -568,7 +522,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -587,7 +541,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -617,7 +571,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -643,7 +597,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -669,7 +623,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -695,7 +649,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -721,7 +675,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -747,7 +701,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -773,7 +727,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -799,7 +753,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -825,7 +779,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -838,15 +792,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -863,7 +811,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -882,7 +830,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -908,7 +856,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -934,7 +882,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -960,7 +908,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -986,7 +934,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1012,7 +960,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1038,7 +986,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1064,7 +1012,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1090,7 +1038,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1116,7 +1064,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1129,15 +1077,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1151,7 +1093,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1170,7 +1112,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1200,7 +1142,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1226,7 +1168,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1252,7 +1194,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1278,7 +1220,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1304,7 +1246,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1330,7 +1272,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1356,7 +1298,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1382,7 +1324,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1408,7 +1350,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1421,592 +1363,616 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="1" customWidth="1"/>
-    <col min="7" max="10" width="10.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.83203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="22.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.1640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="23.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="14.5" style="1"/>
+    <col min="1" max="1" width="21.1719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.67188" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3516" style="1" customWidth="1"/>
+    <col min="8" max="11" width="10.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.8516" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.6719" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.8516" style="1" customWidth="1"/>
+    <col min="16" max="16" width="22.1719" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.1719" style="1" customWidth="1"/>
+    <col min="18" max="18" width="23.5" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="13.75" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" t="s" s="4">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" t="s" s="7">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" t="s" s="7">
         <v>16</v>
       </c>
+      <c r="R1" t="s" s="7">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="6">
+    <row r="2" ht="13.75" customHeight="1">
+      <c r="A2" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B2" s="9">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="D2" s="9">
         <v>111</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10">
+        <v>100</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="M2" s="12">
+        <v>44216</v>
+      </c>
+      <c r="N2" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" ht="13.75" customHeight="1">
+      <c r="A3" t="s" s="7">
         <v>18</v>
       </c>
-      <c r="E2" s="6">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="F2" s="6">
+      <c r="C3" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="D3" s="10">
+        <v>111</v>
+      </c>
+      <c r="E3" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="F3" s="10">
         <v>1</v>
       </c>
-      <c r="G2" s="7">
-        <v>100</v>
-      </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="4" t="s">
+      <c r="G3" s="10">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10">
+        <v>200</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="M3" s="12">
+        <v>44216</v>
+      </c>
+      <c r="N3" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q3" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="R3" t="s" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" ht="13.75" customHeight="1">
+      <c r="A4" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="L2" s="9">
+      <c r="D4" s="10">
+        <v>111</v>
+      </c>
+      <c r="E4" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+      <c r="G4" s="10">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10">
+        <v>110</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="M4" s="12">
         <v>44216</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="4" t="s">
+      <c r="N4" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="O4" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="P4" t="s" s="7">
         <v>24</v>
       </c>
+      <c r="Q4" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="R4" t="s" s="7">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="7">
+    <row r="5" ht="13.75" customHeight="1">
+      <c r="A5" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C5" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="D5" s="10">
         <v>111</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E5" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10">
+        <v>300</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="M5" s="12">
+        <v>44216</v>
+      </c>
+      <c r="N5" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="O5" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="P5" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q5" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="R5" t="s" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" ht="13.75" customHeight="1">
+      <c r="A6" t="s" s="7">
         <v>18</v>
       </c>
-      <c r="E3" s="7">
+      <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="F3" s="7">
+      <c r="C6" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="D6" s="10">
+        <v>111</v>
+      </c>
+      <c r="E6" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="F6" s="10">
+        <v>2</v>
+      </c>
+      <c r="G6" s="10">
+        <v>3</v>
+      </c>
+      <c r="H6" s="10">
+        <v>564</v>
+      </c>
+      <c r="I6" s="10">
+        <v>483</v>
+      </c>
+      <c r="J6" s="10">
+        <v>508</v>
+      </c>
+      <c r="K6" s="11"/>
+      <c r="L6" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="M6" s="12">
+        <v>44216</v>
+      </c>
+      <c r="N6" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="O6" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="P6" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q6" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="R6" t="s" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" ht="13.75" customHeight="1">
+      <c r="A7" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="G3" s="7">
-        <v>200</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="4" t="s">
+      <c r="C7" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="L3" s="9">
+      <c r="D7" s="10">
+        <v>111</v>
+      </c>
+      <c r="E7" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="F7" s="10">
+        <v>2</v>
+      </c>
+      <c r="G7" s="10">
+        <v>3</v>
+      </c>
+      <c r="H7" s="10">
+        <v>673</v>
+      </c>
+      <c r="I7" s="10">
+        <v>573</v>
+      </c>
+      <c r="J7" s="10">
+        <v>584</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="13">
+        <v>44550</v>
+      </c>
+      <c r="M7" s="12">
         <v>44216</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="4" t="s">
+      <c r="N7" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="O7" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="P7" t="s" s="7">
         <v>24</v>
       </c>
+      <c r="Q7" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="R7" t="s" s="7">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="7">
+    <row r="8" ht="13.75" customHeight="1">
+      <c r="A8" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="B8" s="10">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="D8" s="10">
+        <v>222</v>
+      </c>
+      <c r="E8" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="F8" s="10">
+        <v>11</v>
+      </c>
+      <c r="G8" s="10">
+        <v>3</v>
+      </c>
+      <c r="H8" s="10">
+        <v>150</v>
+      </c>
+      <c r="I8" s="10">
+        <v>238</v>
+      </c>
+      <c r="J8" s="10">
+        <v>304</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="M8" s="12">
+        <v>44216</v>
+      </c>
+      <c r="N8" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="O8" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="P8" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q8" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="R8" t="s" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" ht="13.75" customHeight="1">
+      <c r="A9" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="B9" s="10">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="D9" s="10">
+        <v>222</v>
+      </c>
+      <c r="E9" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="F9" s="10">
+        <v>11</v>
+      </c>
+      <c r="G9" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="7">
-        <v>111</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="H9" s="10">
+        <v>238</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="M9" s="12">
+        <v>44216</v>
+      </c>
+      <c r="N9" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="O9" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="P9" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q9" t="s" s="7">
         <v>25</v>
       </c>
-      <c r="E4" s="7">
+      <c r="R9" t="s" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" ht="13.75" customHeight="1">
+      <c r="A10" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="B10" s="10">
         <v>2</v>
       </c>
-      <c r="F4" s="7">
+      <c r="C10" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="D10" s="10">
+        <v>222</v>
+      </c>
+      <c r="E10" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="F10" s="10">
+        <v>22</v>
+      </c>
+      <c r="G10" s="10">
         <v>1</v>
       </c>
-      <c r="G4" s="7">
-        <v>110</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="4" t="s">
+      <c r="H10" s="10">
+        <v>294</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="M10" s="12">
+        <v>44216</v>
+      </c>
+      <c r="N10" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="O10" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="P10" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q10" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="R10" t="s" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" ht="13.75" customHeight="1">
+      <c r="A11" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="B11" s="10">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="L4" s="9">
+      <c r="D11" s="10">
+        <v>222</v>
+      </c>
+      <c r="E11" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="F11" s="10">
+        <v>33</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1</v>
+      </c>
+      <c r="H11" s="10">
+        <v>338</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="M11" s="12">
         <v>44216</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" s="4" t="s">
+      <c r="N11" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="O11" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="P11" t="s" s="7">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7">
-        <v>111</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="Q11" t="s" s="7">
         <v>25</v>
       </c>
-      <c r="E5" s="7">
-        <v>2</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <v>300</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="4" t="s">
+      <c r="R11" t="s" s="7">
         <v>26</v>
-      </c>
-      <c r="L5" s="9">
-        <v>44216</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="7">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7">
-        <v>111</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="7">
-        <v>2</v>
-      </c>
-      <c r="F6" s="7">
-        <v>3</v>
-      </c>
-      <c r="G6" s="7">
-        <v>564</v>
-      </c>
-      <c r="H6" s="7">
-        <v>483</v>
-      </c>
-      <c r="I6" s="7">
-        <v>508</v>
-      </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="9">
-        <v>44216</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7">
-        <v>111</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="7">
-        <v>2</v>
-      </c>
-      <c r="F7" s="7">
-        <v>3</v>
-      </c>
-      <c r="G7" s="7">
-        <v>673</v>
-      </c>
-      <c r="H7" s="7">
-        <v>573</v>
-      </c>
-      <c r="I7" s="7">
-        <v>584</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="10">
-        <v>44550</v>
-      </c>
-      <c r="L7" s="9">
-        <v>44216</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="7">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7">
-        <v>222</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="7">
-        <v>11</v>
-      </c>
-      <c r="F8" s="7">
-        <v>3</v>
-      </c>
-      <c r="G8" s="7">
-        <v>150</v>
-      </c>
-      <c r="H8" s="7">
-        <v>238</v>
-      </c>
-      <c r="I8" s="7">
-        <v>304</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="9">
-        <v>44216</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="7">
-        <v>2</v>
-      </c>
-      <c r="C9" s="7">
-        <v>222</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="7">
-        <v>11</v>
-      </c>
-      <c r="F9" s="7">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7">
-        <v>238</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="9">
-        <v>44216</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="7">
-        <v>2</v>
-      </c>
-      <c r="C10" s="7">
-        <v>222</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="7">
-        <v>22</v>
-      </c>
-      <c r="F10" s="7">
-        <v>1</v>
-      </c>
-      <c r="G10" s="7">
-        <v>294</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" s="9">
-        <v>44216</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="7">
-        <v>2</v>
-      </c>
-      <c r="C11" s="7">
-        <v>222</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="7">
-        <v>33</v>
-      </c>
-      <c r="F11" s="7">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7">
-        <v>338</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" s="9">
-        <v>44216</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
hotfix(condo): DOMA-4532 fixed import meters
</commit_message>
<xml_diff>
--- a/apps/condo/public/meter-import-example.xlsx
+++ b/apps/condo/public/meter-import-example.xlsx
@@ -22,16 +22,16 @@
     <t>Тип помещения</t>
   </si>
   <si>
-    <t>ЛС</t>
+    <t>Лицевой счет</t>
   </si>
   <si>
     <t>Тип счетчика</t>
   </si>
   <si>
-    <t>№ счетчика</t>
-  </si>
-  <si>
-    <t>Кол-во тарифов</t>
+    <t>Номер счетчика</t>
+  </si>
+  <si>
+    <t>Количество тарифов</t>
   </si>
   <si>
     <t>Показание 1</t>
@@ -139,9 +139,9 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="13"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1387,10 +1387,10 @@
     <col min="1" max="1" width="21.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="3.67188" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3516" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1"/>
     <col min="8" max="11" width="10.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="20.8516" style="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" style="1" customWidth="1"/>

</xml_diff>